<commit_message>
Changed clock comparators to dedicated LVDS decoders and changed ADC Vdd inductor to ferrite bead
</commit_message>
<xml_diff>
--- a/BOM_ML605_LPC_Board_wADC_DAC.xlsx
+++ b/BOM_ML605_LPC_Board_wADC_DAC.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TCFH2003\Documents\!!PCB_Projects\ML605_Virtex6_EvalBoard_ExpansionCards\ML605_LPC_Board_wADC_DAC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8775F73A-B0DF-4989-9B88-C806877A0C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FD3DE9-BA7B-4012-A51F-E5FAA4736025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D5F5731A-9380-49D3-BC22-8C4D8C9610F5}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_ML605_LPC_Board_wADC_DAC" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="115">
   <si>
     <t>Reference</t>
   </si>
@@ -160,21 +173,12 @@
     <t>U1,U2</t>
   </si>
   <si>
-    <t>LMV7219M7</t>
-  </si>
-  <si>
     <t>https://www.ti.com/lit/ds/symlink/lmv7219.pdf</t>
   </si>
   <si>
     <t>Package_TO_SOT_SMD:SOT-353_SC-70-5</t>
   </si>
   <si>
-    <t>https://ro.mouser.com/ProductDetail/Texas-Instruments/LMV7219M5X-NOPB?qs=7lkVKPoqpbYs%252BT8enjO7tg%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">926-LMV7219M5X/NOPB </t>
-  </si>
-  <si>
     <t>R40,R41,R42,R43,R44,R45,R46,R47</t>
   </si>
   <si>
@@ -229,30 +233,9 @@
     <t xml:space="preserve">708-RMCF0805FT4K99 </t>
   </si>
   <si>
-    <t>L1</t>
-  </si>
-  <si>
     <t>Inductor_SMD:L_0805_2012Metric_Pad1.05x1.20mm_HandSolder</t>
   </si>
   <si>
-    <t>https://ro.mouser.com/ProductDetail/TAIYO-YUDEN/LBR2012T101K?qs=PzICbMaShUfAbJzk8mcUcA%3D%3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">963-LBR2012T101K </t>
-  </si>
-  <si>
-    <t>JP1,JP2</t>
-  </si>
-  <si>
-    <t>SolderJumper_2_Open</t>
-  </si>
-  <si>
-    <t>Jumper:SolderJumper-2_P1.3mm_Open_TrianglePad1.0x1.5mm</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>J10,J11,J12</t>
   </si>
   <si>
@@ -374,6 +357,27 @@
   </si>
   <si>
     <t>LMH6720MA</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>https://ro.mouser.com/ProductDetail/Bourns/MH2029-471Y?qs=aqFbwuCjQoliK9N17aAXAA%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">652-MH2029-471Y </t>
+  </si>
+  <si>
+    <t>470@100MHz</t>
+  </si>
+  <si>
+    <t>https://ro.mouser.com/ProductDetail/Texas-Instruments/SN65LVDS2DBVR?qs=0le1rQK8zxoNN%2Fzey0Z7qg%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">595-SN65LVDS2DBVR </t>
+  </si>
+  <si>
+    <t>SN65LVDS2DBVR</t>
   </si>
 </sst>
 </file>
@@ -857,9 +861,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1235,10 +1240,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67CD571-2CAB-45BA-9725-FD40A96CE554}">
-  <dimension ref="A1:K28"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,6 +1320,7 @@
         <v>0.69299999999999995</v>
       </c>
       <c r="K2">
+        <f xml:space="preserve"> IF(G2 &lt; 5, G2 * J2, CEILING(G2+1, 5) * J2)</f>
         <v>6.93</v>
       </c>
     </row>
@@ -1347,6 +1353,7 @@
         <v>0.17799999999999999</v>
       </c>
       <c r="K3">
+        <f t="shared" ref="K3:K21" si="0" xml:space="preserve"> IF(G3 &lt; 5, G3 * J3, CEILING(G3+1, 5) * J3)</f>
         <v>2.67</v>
       </c>
     </row>
@@ -1379,6 +1386,7 @@
         <v>0.109</v>
       </c>
       <c r="K4">
+        <f t="shared" si="0"/>
         <v>2.7250000000000001</v>
       </c>
     </row>
@@ -1411,6 +1419,7 @@
         <v>0.46</v>
       </c>
       <c r="K5">
+        <f t="shared" si="0"/>
         <v>0.92</v>
       </c>
     </row>
@@ -1419,7 +1428,7 @@
         <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -1440,6 +1449,7 @@
         <v>10.54</v>
       </c>
       <c r="K6">
+        <f t="shared" si="0"/>
         <v>21.08</v>
       </c>
     </row>
@@ -1469,6 +1479,7 @@
         <v>1.98</v>
       </c>
       <c r="K7">
+        <f t="shared" si="0"/>
         <v>1.98</v>
       </c>
     </row>
@@ -1477,33 +1488,34 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>47</v>
       </c>
-      <c r="D8" t="s">
-        <v>48</v>
-      </c>
       <c r="E8" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="G8">
         <v>2</v>
       </c>
       <c r="I8" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="J8">
-        <v>11.78</v>
+        <v>7.13</v>
       </c>
       <c r="K8">
-        <v>23.56</v>
+        <f t="shared" si="0"/>
+        <v>14.26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>620</v>
@@ -1512,27 +1524,28 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J9">
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="K9">
-        <v>0.84</v>
+        <f t="shared" si="0"/>
+        <v>0.84000000000000008</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B10">
         <v>50</v>
@@ -1541,27 +1554,28 @@
         <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G10">
         <v>8</v>
       </c>
       <c r="I10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J10">
         <v>0.94099999999999995</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
         <v>9.41</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B11">
         <v>39</v>
@@ -1570,362 +1584,349 @@
         <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G11">
         <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J11">
         <v>0.26200000000000001</v>
       </c>
       <c r="K11">
-        <v>6.55</v>
+        <f t="shared" si="0"/>
+        <v>6.5500000000000007</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" t="s">
         <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G12">
         <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="J12">
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="K12">
+        <f t="shared" si="0"/>
         <v>1.1850000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C13" t="s">
         <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E13" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G13">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J13">
         <v>0.46</v>
       </c>
       <c r="K13">
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
+        <v>108</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>111</v>
       </c>
       <c r="C14" t="s">
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>109</v>
       </c>
       <c r="G14">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="J14">
         <v>0.46</v>
       </c>
       <c r="K14">
+        <f t="shared" si="0"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B15" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G15">
-        <v>2</v>
-      </c>
-      <c r="H15" t="s">
-        <v>7</v>
+        <v>3</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15">
+        <v>5.59</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>16.77</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C16" t="s">
         <v>13</v>
       </c>
       <c r="D16" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="G16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I16" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J16">
-        <v>5.59</v>
+        <v>8.51</v>
       </c>
       <c r="K16">
-        <v>16.77</v>
+        <f t="shared" si="0"/>
+        <v>34.04</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J17">
-        <v>8.51</v>
+        <v>0.371</v>
       </c>
       <c r="K17">
-        <v>34.04</v>
+        <f t="shared" si="0"/>
+        <v>3.71</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="I18" t="s">
         <v>87</v>
       </c>
-      <c r="B18" t="s">
-        <v>88</v>
-      </c>
-      <c r="C18" t="s">
-        <v>13</v>
-      </c>
-      <c r="D18" t="s">
-        <v>89</v>
-      </c>
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18">
-        <v>6</v>
-      </c>
-      <c r="I18" t="s">
-        <v>91</v>
-      </c>
       <c r="J18">
-        <v>0.371</v>
+        <v>95.73</v>
       </c>
       <c r="K18">
-        <v>3.71</v>
+        <f t="shared" si="0"/>
+        <v>95.73</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" t="s">
+        <v>91</v>
+      </c>
+      <c r="E19" t="s">
         <v>92</v>
-      </c>
-      <c r="B19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C19" t="s">
-        <v>94</v>
-      </c>
-      <c r="D19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E19" t="s">
-        <v>96</v>
       </c>
       <c r="G19">
         <v>1</v>
       </c>
       <c r="I19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="J19">
-        <v>95.73</v>
+        <v>62.27</v>
       </c>
       <c r="K19">
-        <v>95.73</v>
+        <f t="shared" si="0"/>
+        <v>62.27</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" t="s">
+        <v>97</v>
+      </c>
+      <c r="G20">
+        <v>2</v>
+      </c>
+      <c r="I20" t="s">
         <v>98</v>
       </c>
-      <c r="B20" t="s">
-        <v>99</v>
-      </c>
-      <c r="C20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E20" t="s">
-        <v>102</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="I20" t="s">
-        <v>103</v>
-      </c>
       <c r="J20">
-        <v>62.27</v>
+        <v>15.39</v>
       </c>
       <c r="K20">
-        <v>62.27</v>
+        <f t="shared" si="0"/>
+        <v>30.78</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" t="s">
+        <v>100</v>
+      </c>
+      <c r="C21" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" t="s">
+        <v>91</v>
+      </c>
+      <c r="E21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>103</v>
+      </c>
+      <c r="J21">
+        <v>63.36</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="0"/>
+        <v>63.36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J24" t="s">
         <v>104</v>
       </c>
-      <c r="B21" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" t="s">
-        <v>106</v>
-      </c>
-      <c r="D21" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" t="s">
-        <v>107</v>
-      </c>
-      <c r="G21">
-        <v>2</v>
-      </c>
-      <c r="I21" t="s">
-        <v>108</v>
-      </c>
-      <c r="J21">
-        <v>15.39</v>
-      </c>
-      <c r="K21">
-        <v>30.78</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>109</v>
-      </c>
-      <c r="B22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C22" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" t="s">
-        <v>112</v>
-      </c>
-      <c r="G22">
-        <v>1</v>
-      </c>
-      <c r="I22" t="s">
-        <v>113</v>
-      </c>
-      <c r="J22">
-        <v>63.36</v>
-      </c>
-      <c r="K22">
-        <v>63.36</v>
+      <c r="K24">
+        <f xml:space="preserve"> SUM(K2:K21)</f>
+        <v>376.13</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J25" t="s">
-        <v>114</v>
-      </c>
-      <c r="K25">
-        <v>385.43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J26" t="s">
-        <v>115</v>
-      </c>
-      <c r="K26" s="1">
+        <v>105</v>
+      </c>
+      <c r="K25" s="1">
         <v>0.21</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J28" t="s">
-        <v>116</v>
-      </c>
-      <c r="K28">
-        <v>466.37029999999999</v>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J27" t="s">
+        <v>106</v>
+      </c>
+      <c r="K27">
+        <f xml:space="preserve"> K24 * (1 + K25)</f>
+        <v>455.1173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>